<commit_message>
Updated SomRMWT through new version upload
</commit_message>
<xml_diff>
--- a/Some Rocket Maker Weird Thing.xlsx
+++ b/Some Rocket Maker Weird Thing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1132a9a06cee12/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1611" documentId="8_{085A2D8C-39A3-49E4-8CEE-214FC540B867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{988CC988-707E-4F2F-BB16-172382B5AE67}"/>
+  <xr:revisionPtr revIDLastSave="2413" documentId="8_{085A2D8C-39A3-49E4-8CEE-214FC540B867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1807E17A-87A4-43BA-BE6F-93B22162C3CE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{255BFBE9-9FC6-44F8-AB9D-453C5CE9D40B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Initial Sizing" sheetId="1" r:id="rId3"/>
     <sheet name="Log" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -320,25 +320,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="5">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="5"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="6"/>
+          <xlrd:rvb i="3"/>
         </ext>
       </extLst>
     </bk>
@@ -349,34 +335,18 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="8"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="5">
+  <valueMetadata count="2">
     <bk>
       <rc t="2" v="0"/>
     </bk>
     <bk>
       <rc t="2" v="1"/>
-    </bk>
-    <bk>
-      <rc t="2" v="2"/>
-    </bk>
-    <bk>
-      <rc t="2" v="3"/>
-    </bk>
-    <bk>
-      <rc t="2" v="4"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -401,6 +371,70 @@
   </environmentDefinition>
   <pythonScripts>
     <pythonScript>
+      <code>data_input_df = pd.DataFrame(
+                             data = np.array(xl(%P2%)), 
+                             index = xl(%P3%).squeeze(), 
+                             columns = xl(%P4%).squeeze()
+                             )</code>
+    </pythonScript>
+    <pythonScript>
+      <code>from statistics import geometric_mean
+try: 
+    wadidaw = geometric_mean(data_input_df.loc["Payload", "Primary Mission":"Mission #10"].dropna())
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw</code>
+    </pythonScript>
+    <pythonScript>
+      <code xml:space="preserve">from statistics import geometric_mean
+subset = data_input_df.loc["Assumed ideal single stage delta-v requirement", "Primary Mission":"Mission #10"]
+try: 
+    float_values = subset[subset.apply(lambda x: isinstance(x, float))]
+    wadidaw = geometric_mean(float_values)
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw
+</code>
+    </pythonScript>
+    <pythonScript>
+      <code>from statistics import fmean
+try: 
+    subset = data_input_df.loc["Expected mission orbit inclination", "Primary Mission":"Mission #10"].dropna()
+    wadidaw = fmean(subset)
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw</code>
+    </pythonScript>
+    <pythonScript>
+      <code>from statistics import geometric_mean
+subset = pd.concat([data_input_df.loc["Expected primary launch site latitude", "Primary Mission":"Mission #10"], data_input_df.loc["Expected secondary launch site latitude", "Primary Mission":"Mission #10"]], ignore_index = True)
+try: 
+    float_values = subset[subset.apply(lambda x: isinstance(x, float))]
+    wadidaw = geometric_mean(float_values)
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw</code>
+    </pythonScript>
+    <pythonScript>
+      <code>from statistics import geometric_mean
+subset = data_input_df.loc["Total delta-v needed", "Primary Mission":"Mission #10"]
+try: 
+    float_values = subset[subset.apply(lambda x: isinstance(x, float))]
+    wadidaw = geometric_mean(float_values)
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw</code>
+    </pythonScript>
+    <pythonScript>
+      <code>subset = data_input_df.loc["Total delta-v needed", "Primary Mission":"Mission #10"]
+try: 
+    float_values = subset[subset.apply(lambda x: isinstance(x, float))]
+    wadidaw = np.max(float_values)
+except: 
+    wadidaw = "¯\_(ツ)_/¯"
+wadidaw</code>
+    </pythonScript>
+    <pythonScript>
       <code xml:space="preserve">init_sizing_df = xl(%P2%, headers=True)
 </code>
     </pythonScript>
@@ -416,12 +450,63 @@
     <pythonScript>
       <code>init_sizing_df["Wet mass"][1:xl(%P2%) + 1].sum()</code>
     </pythonScript>
+    <pythonScript>
+      <code>def icikiwir(): 
+    if xl(%P2%) &gt;= xl(%P3%): 
+        return "Yes! OwO"
+    else: 
+        return "No... T_T"
+icikiwir()</code>
+    </pythonScript>
+    <pythonScript>
+      <code>from scipy import optimize
+import math
+import contextlib
+# Initial guesses and parameters
+init_guess = xl(%P2%)
+decision = xl(%P3%)
+pmf = xl(%P4%)
+dmr = xl(%P5%)
+limitations = [pmf, dmr]
+average_delta_v = xl(%P6%)
+max_delta_v = xl(%P7%)
+# Extract last stage parameters as scalars
+last_stage_final_mass = init_sizing_df[init_sizing_df["Stage"] == xl(%P8%)]["Final mass"].astype("float64").values[0]
+last_stage_specimpulse = init_sizing_df[init_sizing_df["Stage"] == xl(%P9%)]["Specific impulse"].astype("float64").values[0]
+# Defining the function to be optimized
+def optimised_function(propratio, dryratio, final_mass, specimpulse):
+    stage_dry_mass = dryratio * final_mass
+    propellant_mass = (propratio * (stage_dry_mass + final_mass)) / (1 - propratio)
+    return 9.81 * specimpulse * math.log((stage_dry_mass + propellant_mass) / stage_dry_mass)
+# Wrapper for optimization to handle a single variable input
+def objective_function(propratio):
+    return -optimised_function(propratio, dmr, last_stage_final_mass, last_stage_specimpulse)
+# Main Loop
+def wakwaw(decision): 
+    if decision == "YES": 
+        # Perform optimization
+        result = optimize.minimize_scalar(objective_function, bounds = (0.01, 0.99), method="bounded", options={"xtol": 1e-10})
+        if result.success:
+            optimized_value = -result.fun  # Negate back to get the actual value
+            if optimized_value &gt;= average_delta_v and optimized_value &gt;= max_delta_v:
+                return optimized_value
+            else:
+                return "Result has not been optimized. Do it again! :D"
+        else:
+            return "Optimization failed."
+    else:
+        return init_guess  # Return initial guess if decision is not "YES"
+# Call the function and store result
+real_result = wakwaw(decision)
+# Output result (you can also set this in a specific cell in Excel)
+real_result</code>
+    </pythonScript>
   </pythonScripts>
 </python>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="199">
   <si>
     <t>Stage</t>
   </si>
@@ -534,9 +619,6 @@
     <t>Stages</t>
   </si>
   <si>
-    <t>Delta-v budget</t>
-  </si>
-  <si>
     <t>HOW TO TABLE</t>
   </si>
   <si>
@@ -586,9 +668,6 @@
   </si>
   <si>
     <t>[MNA]</t>
-  </si>
-  <si>
-    <t>Muhammad Naufal Afif</t>
   </si>
   <si>
     <t>11/01/2025, 23:00 UTC+7</t>
@@ -826,35 +905,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What Even Is This?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SomRMWT is a rocket designer built completely in Excel, designed for hobby rocketry, academic purposes as teaching tool, or conceptual rocket designs. Started when Muhammad Naufal Afif was bored on his sixth year studying aerospace engineering, it provides "good enough" data as baseline for future rocket designs. Currently, it consists of only a rocket initial sizing tool. Contributions from those with expertise or interest in rocketry are highly encouraged to enhance its capabilities.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -912,10 +962,6 @@
     <t>1. Some formatting changes to intro spreadsheet and or Github readme</t>
   </si>
   <si>
-    <t>Pah Hendri
-+6281321210645</t>
-  </si>
-  <si>
     <t>Rocket Name</t>
   </si>
   <si>
@@ -1019,9 +1065,6 @@
   </si>
   <si>
     <t>Total delta-v needed</t>
-  </si>
-  <si>
-    <t>Does it make sense?</t>
   </si>
   <si>
     <t>(Boolean)</t>
@@ -1079,9 +1122,6 @@
     <t>Some Rocket Maker Weird Thing (SomRMWT) - Alpha v0.2 - 13/01/2025</t>
   </si>
   <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Single-stage delta-v for mission</t>
   </si>
   <si>
@@ -1179,6 +1219,155 @@
   </si>
   <si>
     <t>16/01/2025, 16:18 UTC+7</t>
+  </si>
+  <si>
+    <t>1. Uploaded revision to GitHub
+      a.Officially added co-authors
+     b. Refined initial sizing algorithm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What Even Is This?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SomRMWT is a rocket designer built using Excel and coded partially in Python, designed for hobby rocketry, academic purposes as teaching tool, or conceptual rocket designs. Started when Muhammad Naufal Afif was bored on his sixth year studying aerospace engineering, it provides "good enough" data as baseline for future rocket designs. Currently, it consists of a data input sheet and a rocket initial sizing tool. Contributions from those with expertise or interest in rocketry are highly encouraged to enhance its capabilities.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Maximum total delta-v requirement</t>
+  </si>
+  <si>
+    <t>Fulfils average delta-v?</t>
+  </si>
+  <si>
+    <t>Fulfils max delta-v?</t>
+  </si>
+  <si>
+    <t>^ DO NOT EVER TOUCH THIS CELL!!!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">References: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[OwO]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">References: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[OwO]</t>
+    </r>
+  </si>
+  <si>
+    <t>17/01/2025, 16:50 UTC+7</t>
+  </si>
+  <si>
+    <t>1. Improved expected rocket statistics in data input: Now With Python!
+2. Improved log tracking
+3. Improved initial sizing</t>
+  </si>
+  <si>
+    <t>Pak Hendri
++6281321210645</t>
+  </si>
+  <si>
+    <t>DO NOT EVER TOUCH THIS CELL!!! -&gt;</t>
+  </si>
+  <si>
+    <t>Optimise rocket?</t>
+  </si>
+  <si>
+    <t>Optimised delta-v budget</t>
+  </si>
+  <si>
+    <t>Calculated delta-v budget</t>
+  </si>
+  <si>
+    <t>22/01/2025, 16:30 UTC+7</t>
+  </si>
+  <si>
+    <t>1. Revised Python code for data sizing
+2. Switched Python-enabled cell from being Python objects to become Excel values</t>
+  </si>
+  <si>
+    <t>1. "Goal seek" optimisation for rocket initial sizing</t>
+  </si>
+  <si>
+    <t>Graduate
+Aerospace Engineering Study Program, Faculty of Mechanic and Aerospace Engineering
+Institut Teknologi Bandung</t>
+  </si>
+  <si>
+    <t>20/08/2025, 14:20 UTC+7</t>
+  </si>
+  <si>
+    <t>1. Revised lead contributor's position</t>
+  </si>
+  <si>
+    <t>Muhammad Naufal Afif, S.T.</t>
+  </si>
+  <si>
+    <t>[DAS]</t>
+  </si>
+  <si>
+    <t>David Soegijanto, S.T.</t>
+  </si>
+  <si>
+    <t>Graduate Student
+Aerospace Engineering Study Program, Faculty of Mechanic and Aerospace Engineering
+Institut Teknologi Bandung</t>
+  </si>
+  <si>
+    <t>21/08/2025, 21:42 UTC+7</t>
+  </si>
+  <si>
+    <t>1. Added new contributor</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1594,6 +1783,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1610,7 +1802,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="93">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2981,28 +3173,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -3168,7 +3338,152 @@
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="1">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="2">
+  <a r="13" c="11">
+    <v>0</v>
+    <v t="s">Primary Mission</v>
+    <v t="s">Secondary Mission</v>
+    <v t="s">Tertiary Mission</v>
+    <v t="s">Mission #4</v>
+    <v t="s">Mission #5</v>
+    <v t="s">Mission #6</v>
+    <v t="s">Mission #7</v>
+    <v t="s">Mission #8</v>
+    <v t="s">Mission #9</v>
+    <v t="s">Mission #10</v>
+    <v>0</v>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s"/>
+    <v t="s">Payload</v>
+    <v>15000</v>
+    <v>6000</v>
+    <v>10000</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s" xml:space="preserve">What kind of mission? </v>
+    <v t="s">LEO (ISS mission mostly)</v>
+    <v t="s">GEO/GTO</v>
+    <v t="s">MEO</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s" xml:space="preserve">What kind of orbit? </v>
+    <v t="s">Circular</v>
+    <v t="s">Circular</v>
+    <v t="s">Eliptical</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Expected (periapsis) radius</v>
+    <v>6771000</v>
+    <v>42164000</v>
+    <v>28123388</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Expected semi-major axis</v>
+    <v>5000000</v>
+    <v>28123388</v>
+    <v>18758299.796</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">...</v>
+    <v t="s">Expected gimbal angle</v>
+    <v>4</v>
+    <v>4</v>
+    <v>4</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Expected mission orbit inclination</v>
+    <v>0</v>
+    <v>60</v>
+    <v>0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Expected primary launch site latitude</v>
+    <v>7.6466430000000001</v>
+    <v>7.6466430000000001</v>
+    <v>7.6466430000000001</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Expected secondary launch site latitude</v>
+    <v>28.562106</v>
+    <v>28.562106</v>
+    <v>28.562106</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="r">0</v>
+    <v t="s">Total delta-v needed</v>
+    <v>9611.6724427265253</v>
+    <v>18971.879786595753</v>
+    <v>12962.920017163224</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+    <v t="s">Well, that can't happen. Whoops....</v>
+  </a>
   <a r="12" c="12">
     <v t="s"/>
     <v t="s">Stage</v>
@@ -3184,64 +3499,64 @@
     <v t="s">Total delta-v</v>
     <v>0</v>
     <v t="s">Payload</v>
-    <v>9654.8938460562968</v>
+    <v>9654.8938460562986</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v>1</v>
     <v>1</v>
-    <v>9654.8938460562968</v>
-    <v t="s">YES</v>
-    <v t="s">Some weird third thing</v>
-    <v t="s">LOX/HTPB</v>
-    <v t="s">...</v>
-    <v>12472.339333473312</v>
-    <v>30</v>
-    <v>18003333.800354723</v>
-    <v>540100014.01064169</v>
-    <v>12472.339333473312</v>
-    <v>2</v>
-    <v>2</v>
-    <v>96548.938460563004</v>
-    <v t="s">NO</v>
-    <v t="s">Liquid</v>
-    <v t="s">Methalox (LOX/CH4)</v>
-    <v t="s">...</v>
-    <v>6696.8721142085506</v>
-    <v>100</v>
-    <v>29000018.569124788</v>
-    <v>2900001856.9124789</v>
-    <v>19169.211447681861</v>
-    <v>3</v>
-    <v>3</v>
-    <v>965489.38460563018</v>
+    <v>9654.8938460562986</v>
     <v t="s">NO</v>
     <v t="s">Solid</v>
     <v t="s">HTPB (LAPAN)</v>
     <v t="s">...</v>
     <v>4776.7327377850916</v>
-    <v>180</v>
-    <v>114917113.32055132</v>
-    <v>20685080397.699238</v>
-    <v>23945.944185466953</v>
+    <v>30</v>
+    <v>6895026.7992330771</v>
+    <v>206850803.97699231</v>
+    <v>4776.7327377850916</v>
+    <v>2</v>
+    <v>2</v>
+    <v>96548.938460563018</v>
+    <v t="s">NO</v>
+    <v t="s">Solid</v>
+    <v t="s">HTPB (LAPAN)</v>
+    <v t="s">...</v>
+    <v>4776.7327377850916</v>
+    <v>60</v>
+    <v>34475133.996165402</v>
+    <v>2068508039.7699242</v>
+    <v>9553.4654755701831</v>
+    <v>3</v>
+    <v>3</v>
+    <v>965489.38460563053</v>
+    <v t="s">YES</v>
+    <v t="s">Liquid</v>
+    <v t="s">Methalox (LOX/CH4)</v>
+    <v t="s">...</v>
+    <v>7979.2999143768429</v>
+    <v>120</v>
+    <v>287945180.15182835</v>
+    <v>34553421618.219398</v>
+    <v>17532.765389947024</v>
     <v>4</v>
     <v>4</v>
-    <v>9654893.846056303</v>
+    <v>9654893.8460563067</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v t="s">...</v>
     <v t="s">...</v>
     <v t="s">...</v>
@@ -3256,77 +3571,73 @@
     <v t="s">...</v>
     <v>6</v>
     <v>6</v>
-    <v>965489384.60563064</v>
+    <v>965489384.60563123</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v>7</v>
     <v>7</v>
-    <v>9654893846.0563087</v>
+    <v>9654893846.0563145</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v>8</v>
     <v>8</v>
-    <v>96548938460.56311</v>
+    <v>96548938460.563171</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v>9</v>
     <v>9</v>
-    <v>965489384605.63123</v>
+    <v>965489384605.63196</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
     <v>10</v>
     <v>10</v>
-    <v>9654893846056.3145</v>
+    <v>9654893846056.3223</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="r">0</v>
     <v t="s">...</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
-    <v t="r">1</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
+    <v t="r">4</v>
   </a>
 </arrayData>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
   <rv s="0">
     <fb>0</fb>
     <v>2</v>
-  </rv>
-  <rv s="0">
-    <fb>0</fb>
-    <v>3</v>
   </rv>
   <rv s="1">
     <v>0</v>
@@ -3334,60 +3645,45 @@
   <rv s="2">
     <v>DataFrame</v>
     <v>1</v>
-    <v>2</v>
+    <v>1</v>
   </rv>
   <rv s="3">
     <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
     <v>DataFrame</v>
-    <v xml:space="preserve">      Stage    Final mass In vacuum?              Fuel type?  \
-0   Payload  9.654894e+03       None                    None   
-1         1  9.654894e+03        YES  Some weird third thing   
-2         2  9.654894e+04         NO                  Liquid...</v>
+    <v>0                                                        Primary Mission  \
+0                                                                          
+Payload                                                            15000   
+What kind of mission?   ...</v>
+    <v>2</v>
     <v>3</v>
-    <v>4</v>
+  </rv>
+  <rv s="0">
+    <fb>0</fb>
+    <v>6</v>
+  </rv>
+  <rv s="1">
+    <v>1</v>
+  </rv>
+  <rv s="2">
+    <v>DataFrame</v>
+    <v>5</v>
     <v>5</v>
   </rv>
-  <rv s="4">
-    <fb>2</fb>
-    <v>&lt;class 'int'&gt;</v>
-    <v>int</v>
-    <v>2</v>
-    <v>2</v>
-    <v>4</v>
-    <v>5</v>
-  </rv>
-  <rv s="5">
-    <fb>19169.211447681861</fb>
-    <v>&lt;class 'numpy.float64'&gt;</v>
-    <v>float64</v>
-    <v>19169.21144768186</v>
-    <v>19169.211447681861</v>
-    <v>4</v>
-    <v>5</v>
-  </rv>
-  <rv s="5">
-    <fb>10620.38323066193</fb>
-    <v>&lt;class 'numpy.float64'&gt;</v>
-    <v>float64</v>
-    <v>10620.38323066193</v>
-    <v>10620.38323066193</v>
-    <v>4</v>
-    <v>5</v>
-  </rv>
-  <rv s="5">
-    <fb>1062038.3230661931</fb>
-    <v>&lt;class 'numpy.float64'&gt;</v>
-    <v>float64</v>
-    <v>1062038.3230661931</v>
-    <v>1062038.3230661931</v>
-    <v>4</v>
-    <v>5</v>
+  <rv s="3">
+    <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
+    <v>DataFrame</v>
+    <v xml:space="preserve">      Stage    Final mass In vacuum? Fuel type?                Fuel  \
+0   Payload  9.654894e+03       None       None                None   
+1         1  9.654894e+03         NO      Solid        HTPB (LAPAN)   
+2         2  9.654894e+04         NO   ...</v>
+    <v>6</v>
+    <v>3</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
   <s t="_formattednumber">
     <k n="_Format" t="spb"/>
   </s>
@@ -3405,33 +3701,16 @@
     <k n="Python_str" t="s"/>
     <k n="preview" t="r"/>
     <k n="_Provider" t="spb"/>
-    <k n="provider" t="spb"/>
-  </s>
-  <s t="_python">
-    <k n="Python_type" t="s"/>
-    <k n="Python_typeName" t="s"/>
-    <k n="Python_str" t="s"/>
-    <k n="basicValue" t="i"/>
-    <k n="_Provider" t="spb"/>
-    <k n="provider" t="spb"/>
-  </s>
-  <s t="_python">
-    <k n="Python_type" t="s"/>
-    <k n="Python_typeName" t="s"/>
-    <k n="Python_str" t="s"/>
-    <k n="basicValue"/>
-    <k n="_Provider" t="spb"/>
-    <k n="provider" t="spb"/>
   </s>
 </rvStructures>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbData count="6">
+  <spbData count="7">
     <spb s="0">
       <v>11</v>
-      <v>14</v>
+      <v>10</v>
       <v>DataFrame</v>
       <v>arrayPreview</v>
       <v>1</v>
@@ -3442,25 +3721,30 @@
     <spb s="2">
       <v>1</v>
     </spb>
-    <spb s="2">
-      <v>2</v>
-    </spb>
     <spb s="3">
       <v>https://www.anaconda.com/excel</v>
       <v>https://res.cdn.office.net/officepysvc/prod-service/anacondalogo.png</v>
       <v>Python provided by Anaconda</v>
     </spb>
-    <spb s="4">
-      <v>https://www.anaconda.com/excel</v>
-      <v>https://res.cdn.office.net/officepysvc/prod-service/anacondalogo.png</v>
-      <v>Python provided by Anaconda</v>
+    <spb s="0">
+      <v>11</v>
+      <v>14</v>
+      <v>DataFrame</v>
+      <v>arrayPreview</v>
+      <v>1</v>
+    </spb>
+    <spb s="1">
+      <v>4</v>
+    </spb>
+    <spb s="2">
+      <v>2</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="5">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="4">
   <s>
     <k n="drw" t="i"/>
     <k n="dcol" t="i"/>
@@ -3478,11 +3762,6 @@
     <k n="link" t="s"/>
     <k n="logo" t="s"/>
     <k n="name" t="s"/>
-  </s>
-  <s>
-    <k n="url" t="s"/>
-    <k n="logoUrl" t="s"/>
-    <k n="description" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -3509,16 +3788,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{02AC8A23-A629-49DA-9612-16991BC7E0CF}" name="TheDropdownMenuTable_DataInput" displayName="TheDropdownMenuTable_DataInput" ref="B44:F51" totalsRowShown="0" headerRowBorderDxfId="93" tableBorderDxfId="92" totalsRowBorderDxfId="91">
-  <autoFilter ref="B44:F51" xr:uid="{02AC8A23-A629-49DA-9612-16991BC7E0CF}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{37C26436-216C-4530-992E-9414322F8925}" name="Expected Rocket Size (NASA)" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{F7CE6833-F045-4505-BBB1-32CEAA513166}" name="What kind of mission? " dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{2173F227-01D3-4B33-A0D6-EBF6EFF1FD1E}" name="Single-stage delta-v for mission" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{02AC8A23-A629-49DA-9612-16991BC7E0CF}" name="TheDropdownMenuTable_DataInput" displayName="TheDropdownMenuTable_DataInput" ref="B44:E51" totalsRowShown="0" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="B44:E51" xr:uid="{02AC8A23-A629-49DA-9612-16991BC7E0CF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{37C26436-216C-4530-992E-9414322F8925}" name="Expected Rocket Size (NASA)" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{F7CE6833-F045-4505-BBB1-32CEAA513166}" name="What kind of mission? " dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{2173F227-01D3-4B33-A0D6-EBF6EFF1FD1E}" name="Single-stage delta-v for mission" dataDxfId="87">
       <calculatedColumnFormula>((9.81*6378000^3)/(6378000+400000))^0.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1648E833-C30F-405E-9AAA-C8448639848B}" name="What kind of orbit? " dataDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{254C4227-29AA-42F4-8885-BFA9F8CD22D4}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{1648E833-C30F-405E-9AAA-C8448639848B}" name="What kind of orbit? " dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3750,8 +4028,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EF13518-9C68-4392-873C-8B717204DF70}" name="TheDropdownMenuTable_InitialSizing" displayName="TheDropdownMenuTable_InitialSizing" ref="A35:K45" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="A35:K45" xr:uid="{9EF13518-9C68-4392-873C-8B717204DF70}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EF13518-9C68-4392-873C-8B717204DF70}" name="TheDropdownMenuTable_InitialSizing" displayName="TheDropdownMenuTable_InitialSizing" ref="A40:K50" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="A40:K50" xr:uid="{9EF13518-9C68-4392-873C-8B717204DF70}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B53D82EE-C966-4662-82CD-7B051C591F23}" name="Vacuum?" dataDxfId="36"/>
     <tableColumn id="2" xr3:uid="{1F287FF0-02DA-4864-A0EA-D3475D35BA05}" name="Fuel type?" dataDxfId="35"/>
@@ -3774,8 +4052,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB9257BB-A782-4818-94CC-AFB62491CBFD}" name="LogTable" displayName="LogTable" ref="A5:D29" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A5:D29" xr:uid="{CB9257BB-A782-4818-94CC-AFB62491CBFD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB9257BB-A782-4818-94CC-AFB62491CBFD}" name="LogTable" displayName="LogTable" ref="A5:D155" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A5:D155" xr:uid="{CB9257BB-A782-4818-94CC-AFB62491CBFD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2A328167-11A1-4BEB-9A4A-A7784AD4ED68}" name="Date and Time" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{5B0BF100-708E-454B-80A0-E23284DA6871}" name="Who?*" dataDxfId="19"/>
@@ -4121,61 +4399,61 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.21875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="42" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="72" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4185,10 +4463,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15981B98-6F6F-4F60-9883-7D14D06EDCA5}">
-  <dimension ref="B2:L61"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="B2:L63"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4200,7 +4479,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="54"/>
     </row>
@@ -4210,36 +4489,36 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C7" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C9" s="11">
         <v>6</v>
@@ -4247,7 +4526,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C10" s="11">
         <v>0.01</v>
@@ -4255,37 +4534,37 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="G13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -4311,16 +4590,16 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
@@ -4332,16 +4611,16 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
@@ -4353,17 +4632,17 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="44" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C17" s="11">
         <v>6771000</v>
       </c>
       <c r="D17" s="11">
-        <v>11371000</v>
+        <v>42164000</v>
       </c>
       <c r="E17" s="34">
-        <f>6378000+1500000</f>
-        <v>7878000</v>
+        <f>0.667*DataInputTable[[#This Row],[Secondary Mission]]</f>
+        <v>28123388</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -4375,17 +4654,18 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C18" s="11">
         <v>5000000</v>
       </c>
       <c r="D18" s="11">
-        <v>45000000</v>
+        <f>0.667*D17</f>
+        <v>28123388</v>
       </c>
       <c r="E18" s="34">
         <f>0.667*E17</f>
-        <v>5254626</v>
+        <v>18758299.796</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -4397,7 +4677,7 @@
     </row>
     <row r="19" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="44" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C19" s="40">
         <f>IF(
@@ -4459,7 +4739,7 @@
                     )
                )
 )</f>
-        <v>8368.6957072771529</v>
+        <v>10741.65441050474</v>
       </c>
       <c r="E19" s="37">
         <f>IF(
@@ -4490,7 +4770,7 @@
                     )
                )
 )</f>
-        <v>5036.4131222932047</v>
+        <v>10334.196520863028</v>
       </c>
       <c r="F19" s="37" t="str">
         <f>IF(
@@ -4712,7 +4992,7 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="44" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C20" s="11">
         <v>4</v>
@@ -4733,13 +5013,13 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="44" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C21" s="11">
         <v>0</v>
       </c>
       <c r="D21" s="11">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E21" s="34">
         <v>0</v>
@@ -4754,7 +5034,7 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11">
         <v>7.6466430000000001</v>
@@ -4775,7 +5055,7 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="44" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C23" s="11">
         <v>28.562106</v>
@@ -4796,7 +5076,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="44" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <f>IFERROR(
@@ -4820,11 +5100,11 @@
     ),
     "Well, that can't happen. Whoops...."
 )</f>
-        <v>10491.854787858914</v>
+        <v>18971.879786595753</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="0"/>
-        <v>6302.4451953777252</v>
+        <v>12962.920017163224</v>
       </c>
       <c r="F24" s="5" t="str">
         <f t="shared" si="0"/>
@@ -4855,207 +5135,218 @@
         <v>Well, that can't happen. Whoops....</v>
       </c>
     </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H26" t="e" cm="1" vm="1">
+        <f t="array" ref="H26">_xlfn._xlws.PY(0,1,DataInputTable[[Primary Mission]:[Mission '#10]],DataInputTable[Attribute],DataInputTable[[#Headers],[Primary Mission]:[Mission '#10]])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E27" s="55" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F27" s="56"/>
       <c r="G27" s="57"/>
+      <c r="H27" s="39" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E28" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="5">
-        <f>GEOMEAN(C14:L14)</f>
-        <v>9654.8938460562968</v>
+        <v>126</v>
+      </c>
+      <c r="F28" s="5" cm="1">
+        <f t="array" ref="F28">_xlfn._xlws.PY(1,0)</f>
+        <v>9654.8938460562986</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E29" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F29" s="5">
-        <f>IFERROR(GEOMEAN(C19:L19), "¯\_(ツ)_/¯")</f>
-        <v>6862.751528224343</v>
+        <v>143</v>
+      </c>
+      <c r="F29" s="5" cm="1">
+        <f t="array" ref="F29">_xlfn._xlws.PY(2,0)</f>
+        <v>9477.3706242110438</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E30" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="5">
-        <f>AVERAGE(C21:L21)</f>
-        <v>0</v>
+        <v>166</v>
+      </c>
+      <c r="F30" s="5" cm="1">
+        <f t="array" ref="F30">_xlfn._xlws.PY(3,0)</f>
+        <v>20</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E31" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="5">
-        <f>IFERROR(GEOMEAN(C22:L22, C23:L23), "¯\_(ツ)_/¯")</f>
+        <v>127</v>
+      </c>
+      <c r="F31" s="5" cm="1">
+        <f t="array" ref="F31">_xlfn._xlws.PY(4,0)</f>
         <v>14.778505604767959</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E32" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="5">
-        <f>IFERROR(GEOMEAN(C24:L24), "¯\_(ツ)_/¯")</f>
-        <v>8597.7887528933989</v>
+        <v>128</v>
+      </c>
+      <c r="F32" s="5" cm="1">
+        <f t="array" ref="F32">_xlfn._xlws.PY(5,0)</f>
+        <v>13321.017203557933</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F33" s="5" cm="1">
+        <f t="array" ref="F33">_xlfn._xlws.PY(6,0)</f>
+        <v>18971.879786595753</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D35" s="33"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="53"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="39"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D45" s="5">
         <f>IFERROR(((9.81*6371000^2)/(INDEX($C$17:$L$17, (MATCH("LEO (ISS mission mostly)", $C$15:$L$15, 0)))))^0.5, ((9.81*6371000^2)/(6378000+400000))^0.5)</f>
         <v>7668.5932308350311</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D46" s="5">
         <f>IFERROR($D$45+((9.81*6371000^2)/(INDEX($C$17:$L$17,(MATCH("MEO",$C$15:$L$15,0)))))^0.5, $D$45+((9.81*6371000^2)/(6378000+AVERAGE(1000000, 35786000)))^0.5)</f>
-        <v>14778.012394817439</v>
+        <v>11431.368573829686</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D47" s="5">
         <f>IFERROR($D$45+((9.81*6371000^2)/(INDEX($C$17:$L$17,(MATCH("GEO/GTO",$C$15:$L$15,0)))))^0.5, $D$45+((9.81*6371000^2)/42164000)^0.5)</f>
-        <v>13586.154715137456</v>
+        <v>10741.65441050474</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D48" s="5">
         <f>$D$45+3200+900</f>
         <v>11768.593230835031</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>155</v>
+      </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D49" s="5">
         <f>$D$45+4300+900</f>
         <v>12868.593230835031</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>120</v>
+      </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D50" s="5">
         <f>$D$45 + GEOMEAN(5500, 3500) + 900</f>
         <v>12956.075424531093</v>
       </c>
       <c r="E50" s="6"/>
-      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D51" s="5">
         <f>$D$45 + GEOMEAN(6300, 7300, 8000, 8200, 8200) + 900</f>
         <v>16131.281864605833</v>
       </c>
       <c r="E51" s="9"/>
-      <c r="F51" s="5"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="51" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C53" s="52"/>
       <c r="D53" s="52"/>
@@ -5065,24 +5356,24 @@
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="38" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C55" s="5">
         <f t="shared" ref="C55:C61" si="1">D45</f>
@@ -5122,60 +5413,60 @@
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C56" s="5">
         <f>D46</f>
-        <v>14778.012394817439</v>
+        <v>11431.368573829686</v>
       </c>
       <c r="D56" s="42">
-        <f>IFERROR(
+        <f>IFERROR($D$45 +
     ((9.81 * (6378000 ^ 2)) *
         (
             (2 / INDEX($C$17:$L$17, MATCH("MEO", $C$15:$L$15, 0))) -
             (1 / INDEX($C$18:$L$18, MATCH("MEO", $C$15:$L$15, 0)))
         )
-    ) ^ 0.5,
+    ) ^ 0.5, $D$45 +
     ((9.81 * (6378000 ^ 2)) *
         (
-            (2 / (6378000 + AVERAGE(1000000,35786000))) -
-            (1 / (0.667 * (6378000 + AVERAGE(1000000,35786000))))
+            (2 / (6378000 + AVERAGE(1000000, 35786000))) -
+            (1 / (0.667 * (6378000 + AVERAGE(1000000, 35786000))))
         )
     ) ^ 0.5
 )</f>
-        <v>5036.4131222932047</v>
+        <v>10334.196520863028</v>
       </c>
       <c r="E56" s="5">
         <f>IFERROR(
     ((2 * 9.81 * (6371000 ^ 2)) / INDEX($C$17:$L$17, MATCH("MEO", $C$15:$L$15, 0))) ^ 0.5,
     ((2 * 9.81 * (6371000 ^ 2)) / (6371000 + AVERAGE(1000000,35786000))) ^ 0.5
 )</f>
-        <v>10054.237002299111</v>
+        <v>5321.3679222261162</v>
       </c>
       <c r="F56" s="5">
         <f>IFERROR(
     ((2 * 9.81 * (6371000 ^ 2)) / INDEX($C$17:$L$17, MATCH("MEO", $C$15:$L$15, 0)) + 1000^2) ^ 0.5,
     (((2 * 9.81 * (6371000 ^ 2)) / (6371000 + AVERAGE(1000000,35786000))) + 1000^2) ^ 0.5
 )</f>
-        <v>10103.844896790559</v>
+        <v>5414.513511267387</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C57" s="5">
         <f t="shared" si="1"/>
-        <v>13586.154715137456</v>
+        <v>10741.65441050474</v>
       </c>
       <c r="D57" s="42">
-        <f>IFERROR(
+        <f>IFERROR($D$45 +
     ((9.81 * (6378000 ^ 2)) *
         (
             (2 / INDEX($C$17:$L$17, MATCH("GEO/GTO", $C$15:$L$15, 0))) -
             (1 / INDEX($C$18:$L$18, MATCH("GEO/GTO", $C$15:$L$15, 0)))
         )
-    ) ^ 0.5,
+    ) ^ 0.5, $D$45 +
     ((9.81 * (6378000 ^ 2)) *
         (
             (2 / (42164000)) -
@@ -5183,101 +5474,106 @@
         )
     ) ^ 0.5
 )</f>
-        <v>7830.7761263937309</v>
+        <v>9845.5932492484426</v>
       </c>
       <c r="E57" s="5">
         <f>IFERROR(
     ((2 * 9.81 * (6371000 ^ 2)) / INDEX($C$17:$L$17, MATCH("GEO/GTO", $C$15:$L$15, 0))) ^ 0.5,
     ((2 * 9.81 * (6371000 ^ 2)) / (42164000)) ^ 0.5
 )</f>
-        <v>8368.6957072771529</v>
+        <v>4345.9647982911647</v>
       </c>
       <c r="F57" s="5">
         <f>IFERROR(
     ((2 * 9.81 * (6371000 ^ 2)) / INDEX($C$17:$L$17, MATCH("GEO/GTO", $C$15:$L$15, 0)) + 1000^2) ^ 0.5,
     (((2 * 9.81 * (6371000 ^ 2)) / (42164000)) + 1000^2) ^ 0.5
 )</f>
-        <v>8428.2304098190762</v>
+        <v>4459.5302474572318</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C58" s="5">
         <f t="shared" si="1"/>
         <v>11768.593230835031</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C59" s="5">
         <f t="shared" si="1"/>
         <v>12868.593230835031</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C60" s="5">
         <f t="shared" si="1"/>
         <v>12956.075424531093</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C61" s="8">
         <f t="shared" si="1"/>
         <v>16131.281864605833</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="39" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B43:F43"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B43:E43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
@@ -5292,14 +5588,15 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F15" calculatedColumn="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="3">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5307,24 +5604,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BF2A92-EDB0-493F-BE9F-61B52BCD98C8}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A4" zoomScale="79" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -5333,7 +5630,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="54"/>
     </row>
@@ -5343,12 +5640,12 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C5" s="11">
         <v>0.9</v>
@@ -5356,7 +5653,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C6" s="11">
         <v>0.1</v>
@@ -5382,7 +5679,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>30</v>
@@ -5412,7 +5709,7 @@
       </c>
       <c r="B10" s="5">
         <f>'Data Input'!$F$28</f>
-        <v>9654.8938460562968</v>
+        <v>9654.8938460562986</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -5420,7 +5717,7 @@
       <c r="F10" s="36"/>
       <c r="G10" s="5">
         <f>B10</f>
-        <v>9654.8938460562968</v>
+        <v>9654.8938460562986</v>
       </c>
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
@@ -5436,51 +5733,51 @@
       </c>
       <c r="B11" s="5">
         <f>G10</f>
-        <v>9654.8938460562968</v>
+        <v>9654.8938460562986</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F11" s="5">
         <f>IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Solid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (solid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (solid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (solid)], 0)), IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Liquid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (liquid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (liquid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (liquid)], 0)), INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (IDFK, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (IDFK, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (IDFK)], 0))))</f>
-        <v>576</v>
+        <v>220.6</v>
       </c>
       <c r="G11" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>965.48938460562977</v>
+        <v>965.48938460562988</v>
       </c>
       <c r="H11" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>95583.449075957367</v>
+        <v>95583.449075957382</v>
       </c>
       <c r="I11" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>96548.938460563004</v>
+        <v>96548.938460563018</v>
       </c>
       <c r="J11" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
-        <v>12472.339333473312</v>
+        <v>4776.7327377850916</v>
       </c>
       <c r="K11" s="11">
         <v>30</v>
       </c>
       <c r="L11" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*(LeInitialSizingTable[[#This Row],[Propellant mass]]/LeInitialSizingTable[[#This Row],[Burn time]])</f>
-        <v>18003333.800354723</v>
+        <v>6895026.7992330771</v>
       </c>
       <c r="M11" s="5">
         <f>LeInitialSizingTable[[#This Row],[Thrust]]*LeInitialSizingTable[[#This Row],[Burn time]]</f>
-        <v>540100014.01064169</v>
+        <v>206850803.97699231</v>
       </c>
       <c r="N11" s="6">
         <f>SUM(J11)</f>
-        <v>12472.339333473312</v>
+        <v>4776.7327377850916</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -5489,51 +5786,51 @@
       </c>
       <c r="B12" s="5">
         <f>I11</f>
-        <v>96548.938460563004</v>
+        <v>96548.938460563018</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5">
         <f>IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Solid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (solid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (solid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (solid)], 0)), IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Liquid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (liquid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (liquid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (liquid)], 0)), INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (IDFK, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (IDFK, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (IDFK)], 0))))</f>
-        <v>309.27625</v>
+        <v>220.6</v>
       </c>
       <c r="G12" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>9654.8938460563004</v>
+        <v>9654.8938460563022</v>
       </c>
       <c r="H12" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>955834.49075957388</v>
+        <v>955834.49075957423</v>
       </c>
       <c r="I12" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>965489.38460563018</v>
+        <v>965489.38460563053</v>
       </c>
       <c r="J12" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
-        <v>6696.8721142085506</v>
+        <v>4776.7327377850916</v>
       </c>
       <c r="K12" s="11">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L12" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*(LeInitialSizingTable[[#This Row],[Propellant mass]]/LeInitialSizingTable[[#This Row],[Burn time]])</f>
-        <v>29000018.569124788</v>
+        <v>34475133.996165402</v>
       </c>
       <c r="M12" s="5">
         <f>LeInitialSizingTable[[#This Row],[Thrust]]*LeInitialSizingTable[[#This Row],[Burn time]]</f>
-        <v>2900001856.9124789</v>
+        <v>2068508039.7699242</v>
       </c>
       <c r="N12" s="6">
         <f>SUM($J$11:J12)</f>
-        <v>19169.211447681861</v>
+        <v>9553.4654755701831</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -5542,51 +5839,51 @@
       </c>
       <c r="B13" s="5">
         <f>I12</f>
-        <v>965489.38460563018</v>
+        <v>965489.38460563053</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F13" s="5">
         <f>IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Solid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (solid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (solid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (solid)], 0)), IF(LeInitialSizingTable[[#This Row],[Fuel type?]] = "Liquid", INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (liquid, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (liquid, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (liquid)], 0)), INDEX(IF(LeInitialSizingTable[[#This Row],[In vacuum?]] = "YES", TheDropdownMenuTable_InitialSizing[Isp (IDFK, vacuum)], TheDropdownMenuTable_InitialSizing[Isp (IDFK, SL)]), MATCH(LeInitialSizingTable[[#This Row],[Fuel]], TheDropdownMenuTable_InitialSizing[Fuel (IDFK)], 0))))</f>
-        <v>220.6</v>
+        <v>368.50157999999999</v>
       </c>
       <c r="G13" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>96548.938460563018</v>
+        <v>96548.938460563062</v>
       </c>
       <c r="H13" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>9558344.9075957406</v>
+        <v>9558344.9075957444</v>
       </c>
       <c r="I13" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>9654893.846056303</v>
+        <v>9654893.8460563067</v>
       </c>
       <c r="J13" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
-        <v>4776.7327377850916</v>
+        <v>7979.2999143768429</v>
       </c>
       <c r="K13" s="11">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="L13" s="5">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*(LeInitialSizingTable[[#This Row],[Propellant mass]]/LeInitialSizingTable[[#This Row],[Burn time]])</f>
-        <v>114917113.32055132</v>
+        <v>287945180.15182835</v>
       </c>
       <c r="M13" s="5">
         <f>LeInitialSizingTable[[#This Row],[Thrust]]*LeInitialSizingTable[[#This Row],[Burn time]]</f>
-        <v>20685080397.699238</v>
+        <v>34553421618.219398</v>
       </c>
       <c r="N13" s="6">
         <f>SUM($J$11:J13)</f>
-        <v>23945.944185466953</v>
+        <v>17532.765389947024</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -5595,7 +5892,7 @@
       </c>
       <c r="B14" s="5">
         <f t="shared" ref="B14:B20" si="0">I13</f>
-        <v>9654893.846056303</v>
+        <v>9654893.8460563067</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -5606,15 +5903,15 @@
       </c>
       <c r="G14" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>965489.3846056303</v>
+        <v>965489.38460563077</v>
       </c>
       <c r="H14" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>95583449.075957403</v>
+        <v>95583449.075957462</v>
       </c>
       <c r="I14" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>96548938.460563034</v>
+        <v>96548938.460563093</v>
       </c>
       <c r="J14" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5640,7 +5937,7 @@
       </c>
       <c r="B15" s="5">
         <f t="shared" si="0"/>
-        <v>96548938.460563034</v>
+        <v>96548938.460563093</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -5651,15 +5948,15 @@
       </c>
       <c r="G15" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>9654893.846056303</v>
+        <v>9654893.8460563105</v>
       </c>
       <c r="H15" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>955834490.75957429</v>
+        <v>955834490.75957489</v>
       </c>
       <c r="I15" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>965489384.60563064</v>
+        <v>965489384.60563123</v>
       </c>
       <c r="J15" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5685,7 +5982,7 @@
       </c>
       <c r="B16" s="5">
         <f t="shared" si="0"/>
-        <v>965489384.60563064</v>
+        <v>965489384.60563123</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5696,15 +5993,15 @@
       </c>
       <c r="G16" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>96548938.460563064</v>
+        <v>96548938.460563123</v>
       </c>
       <c r="H16" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>9558344907.5957451</v>
+        <v>9558344907.5957508</v>
       </c>
       <c r="I16" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>9654893846.0563087</v>
+        <v>9654893846.0563145</v>
       </c>
       <c r="J16" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5730,7 +6027,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" si="0"/>
-        <v>9654893846.0563087</v>
+        <v>9654893846.0563145</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -5741,15 +6038,15 @@
       </c>
       <c r="G17" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>965489384.60563087</v>
+        <v>965489384.60563147</v>
       </c>
       <c r="H17" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>95583449075.957474</v>
+        <v>95583449075.957535</v>
       </c>
       <c r="I17" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>96548938460.56311</v>
+        <v>96548938460.563171</v>
       </c>
       <c r="J17" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5775,7 +6072,7 @@
       </c>
       <c r="B18" s="5">
         <f t="shared" si="0"/>
-        <v>96548938460.56311</v>
+        <v>96548938460.563171</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -5786,15 +6083,15 @@
       </c>
       <c r="G18" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>9654893846.0563107</v>
+        <v>9654893846.0563183</v>
       </c>
       <c r="H18" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>955834490759.57495</v>
+        <v>955834490759.57568</v>
       </c>
       <c r="I18" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>965489384605.63123</v>
+        <v>965489384605.63196</v>
       </c>
       <c r="J18" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5820,7 +6117,7 @@
       </c>
       <c r="B19" s="5">
         <f t="shared" si="0"/>
-        <v>965489384605.63123</v>
+        <v>965489384605.63196</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -5831,15 +6128,15 @@
       </c>
       <c r="G19" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>96548938460.563126</v>
+        <v>96548938460.563202</v>
       </c>
       <c r="H19" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>9558344907595.752</v>
+        <v>9558344907595.7598</v>
       </c>
       <c r="I19" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>9654893846056.3145</v>
+        <v>9654893846056.3223</v>
       </c>
       <c r="J19" s="5" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5865,9 +6162,9 @@
       </c>
       <c r="B20" s="5">
         <f t="shared" si="0"/>
-        <v>9654893846056.3145</v>
-      </c>
-      <c r="C20" s="8"/>
+        <v>9654893846056.3223</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="e">
@@ -5876,15 +6173,15 @@
       </c>
       <c r="G20" s="5">
         <f>$C$6*LeInitialSizingTable[[#This Row],[Final mass]]</f>
-        <v>965489384605.63147</v>
+        <v>965489384605.63232</v>
       </c>
       <c r="H20" s="5">
         <f>($C$5*(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))/(1-$C$5)</f>
-        <v>95583449075957.547</v>
+        <v>95583449075957.625</v>
       </c>
       <c r="I20" s="5">
         <f>LeInitialSizingTable[[#This Row],[Propellant mass]] + LeInitialSizingTable[[#This Row],[Stage dry mass]]</f>
-        <v>96548938460563.172</v>
+        <v>96548938460563.25</v>
       </c>
       <c r="J20" s="8" t="e">
         <f>9.81*LeInitialSizingTable[[#This Row],[Specific impulse]]*LN(LeInitialSizingTable[[#This Row],[Wet mass]]/(LeInitialSizingTable[[#This Row],[Stage dry mass]]+LeInitialSizingTable[[#This Row],[Final mass]]))</f>
@@ -5916,377 +6213,445 @@
       <c r="N21" s="45"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I23" t="e" cm="1" vm="1">
-        <f t="array" ref="I23">_xlfn._xlws.PY(0,1,LeInitialSizingTable[#All])</f>
+      <c r="G23" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="I23" t="e" cm="1" vm="2">
+        <f t="array" ref="I23">_xlfn._xlws.PY(7,1,LeInitialSizingTable[#All])</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F24" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
+      <c r="F24" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="5" cm="1" vm="2">
-        <f t="array" ref="G25">_xlfn._xlws.PY(1,1,'Data Input'!$C$7)</f>
-        <v>2</v>
+      <c r="G25" s="5" cm="1">
+        <f t="array" ref="G25">_xlfn._xlws.PY(8,0,'Data Input'!$C$7)</f>
+        <v>3</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="5" cm="1" vm="3">
-        <f t="array" ref="G26">_xlfn._xlws.PY(2,1,$G$25)</f>
-        <v>19169.211447681861</v>
+        <v>186</v>
+      </c>
+      <c r="G26" s="5" cm="1">
+        <f t="array" ref="G26">_xlfn._xlws.PY(9,0,$G$25)</f>
+        <v>17532.765389947024</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="5" cm="1" vm="4">
-        <f t="array" ref="G27">_xlfn._xlws.PY(3,1,$G$25)</f>
-        <v>10620.38323066193</v>
+        <v>44</v>
+      </c>
+      <c r="G27" s="5" cm="1">
+        <f t="array" ref="G27">_xlfn._xlws.PY(10,0,$G$25)</f>
+        <v>107169.32169122499</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F28" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G28" s="5" cm="1" vm="5">
-        <f t="array" ref="G28">_xlfn._xlws.PY(4,1,$G$25)</f>
-        <v>1062038.3230661931</v>
+        <v>159</v>
+      </c>
+      <c r="G28" s="5" cm="1">
+        <f t="array" ref="G28">_xlfn._xlws.PY(11,0,$G$25)</f>
+        <v>10716932.1691225</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F29" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G29" s="5" t="str">
-        <f>IF(MAX($G$26, 'Data Input'!$F$32) = $G$26, "Yes! OwO", "No... T_T")</f>
+        <v>175</v>
+      </c>
+      <c r="G29" s="5" t="str" cm="1">
+        <f t="array" ref="G29">_xlfn._xlws.PY(12,0,$G$26,'Data Input'!$F$32)</f>
         <v>Yes! OwO</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F30" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="5" t="str" cm="1">
+        <f t="array" ref="G30">_xlfn._xlws.PY(12,0,$G$26,'Data Input'!$F$33)</f>
+        <v>No... T_T</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="54"/>
       <c r="C31" s="41"/>
+      <c r="F31" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A32" s="41"/>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
+      <c r="F32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G32" s="5" cm="1">
+        <f t="array" ref="G32">_xlfn._xlws.PY(13,0,$G$26,$G$31,$C$5,$C$6,'Data Input'!$F$32,'Data Input'!$F$33,'Data Input'!$C$7,'Data Input'!$C$7)</f>
+        <v>25280.940689105093</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
+      <c r="F33" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" s="5" t="str" cm="1">
+        <f t="array" ref="G33">_xlfn._xlws.PY(12,0,$G$32,'Data Input'!$F$32)</f>
+        <v>Yes! OwO</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F34" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="5" t="str" cm="1">
+        <f t="array" ref="G34">_xlfn._xlws.PY(12,0,$G$32,'Data Input'!$F$33)</f>
+        <v>Yes! OwO</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="54"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B40" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C40" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D40" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E40" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F40" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G40" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H40" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I35" s="26" t="s">
+      <c r="I40" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J40" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="K35" s="27" t="s">
+      <c r="K40" s="27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B41" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C41" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="44">
+      <c r="D41" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (solid, SL)]]</f>
         <v>330.9</v>
       </c>
-      <c r="E36" s="44">
+      <c r="E41" s="44">
         <f>AVERAGE(220, 220, 220, 203, 240)</f>
         <v>220.6</v>
       </c>
-      <c r="F36" s="44" t="s">
+      <c r="F41" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="44">
+      <c r="G41" s="44">
         <v>454.84199999999998</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H41" s="44">
         <v>388.78694999999999</v>
       </c>
-      <c r="I36" s="44" t="s">
+      <c r="I41" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="J36" s="44">
+      <c r="J41" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (IDFK, SL)]]</f>
         <v>315</v>
       </c>
-      <c r="K36" s="47">
+      <c r="K41" s="47">
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B42" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C42" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="44">
+      <c r="D42" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (solid, SL)]]</f>
         <v>244.12199999999999</v>
       </c>
-      <c r="E37" s="44">
+      <c r="E42" s="44">
         <v>162.74799999999999</v>
       </c>
-      <c r="F37" s="44" t="s">
+      <c r="F42" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="44">
+      <c r="G42" s="44">
         <v>368.50157999999999</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H42" s="44">
         <v>309.27625</v>
       </c>
-      <c r="I37" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="J37" s="44">
+      <c r="I42" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="J42" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (IDFK, SL)]]</f>
         <v>337.5</v>
       </c>
-      <c r="K37" s="47">
+      <c r="K42" s="47">
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
-      <c r="B38" s="44" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="46"/>
+      <c r="B43" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C43" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="44">
+        <v>285.60000000000002</v>
+      </c>
+      <c r="E43" s="44">
+        <v>242</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="44">
+        <v>357.79817000000003</v>
+      </c>
+      <c r="H43" s="44">
+        <v>299.79613000000001</v>
+      </c>
+      <c r="I43" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="44">
-        <v>285.60000000000002</v>
-      </c>
-      <c r="E38" s="44">
-        <v>242</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="44">
-        <v>357.79817000000003</v>
-      </c>
-      <c r="H38" s="44">
-        <v>299.79613000000001</v>
-      </c>
-      <c r="I38" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="J38" s="44">
+      <c r="J43" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (IDFK, SL)]]</f>
         <v>576</v>
       </c>
-      <c r="K38" s="47">
+      <c r="K43" s="47">
         <v>384</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="44">
+    <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="46"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="44">
         <f>1.5*TheDropdownMenuTable_InitialSizing[[#This Row],[Isp (solid, SL)]]</f>
         <v>116.25</v>
       </c>
-      <c r="E39" s="44">
+      <c r="E44" s="44">
         <v>77.5</v>
       </c>
-      <c r="F39" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="44">
+      <c r="F44" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G44" s="44">
         <v>341.38634000000002</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H44" s="44">
         <v>288.58308</v>
       </c>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="47"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="44">
-        <v>333</v>
-      </c>
-      <c r="H40" s="44">
-        <v>285</v>
-      </c>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="47"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="46"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="44">
-        <v>343.42507999999998</v>
-      </c>
-      <c r="H41" s="44">
-        <v>291.74311999999998</v>
-      </c>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="47"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="44">
-        <v>341.18247000000002</v>
-      </c>
-      <c r="H42" s="44">
-        <v>288.17532999999997</v>
-      </c>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="47"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="46"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="47"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
       <c r="I44" s="44"/>
       <c r="J44" s="44"/>
       <c r="K44" s="47"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="50"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="44">
+        <v>333</v>
+      </c>
+      <c r="H45" s="44">
+        <v>285</v>
+      </c>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="47"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="46"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="44">
+        <v>343.42507999999998</v>
+      </c>
+      <c r="H46" s="44">
+        <v>291.74311999999998</v>
+      </c>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="47"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="46"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="44">
+        <v>341.18247000000002</v>
+      </c>
+      <c r="H47" s="44">
+        <v>288.17532999999997</v>
+      </c>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="47"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="46"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="47"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="46"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="47"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="48"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="50"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="F24:H24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="WTF" error="What are you doing? Insert valid data!" promptTitle="Fuel type" prompt="Please select fuel type" sqref="D11:D20" xr:uid="{75774DDE-7B63-4B96-895A-4AEB3A1915AC}">
-      <formula1>$B$36:$B$38</formula1>
+      <formula1>$B$41:$B$43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Huh?" error="Did you input that correctly? Insert valid data" promptTitle="Can haz vacuum?" prompt="Pleas input stage condition in use" sqref="C11:C20" xr:uid="{27B2952E-10CB-495C-8AE7-7BD4B0C75E94}">
-      <formula1>$A$36:$A$37</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Huh?" error="Did you input that correctly? Insert valid data" promptTitle="Can haz vacuum?" prompt="Please input stage condition in use" sqref="C11:C20" xr:uid="{B85ED1B4-F14F-489F-B136-53C345B9CC66}">
+      <formula1>$A$41:$A$42</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Huh?" error="Did you input that correctly? Insert valid data" promptTitle="Wanna optimise rocket?" prompt="Change this cell to activate the Python code to &quot;goal seek&quot; the rocket such that all delta-v requirements are met" sqref="G31" xr:uid="{FE49B061-2D2A-4848-A0E9-84581B614EE7}">
+      <formula1>$A$41:$A$42</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="NOT AGAIN" error="What even?! Please insert valid data!" promptTitle="Fuel type 2: Electric Boogaloo" prompt="Please specify fuel type" sqref="E11:E20" xr:uid="{D3232489-5E3A-4360-884B-9C39225CAB94}">
-      <formula1>IF($D11 = "Solid", $C$36:$C$45, IF($D11 = "Liquid", $F$36:$F$45, $I$36:$I$45))</formula1>
+      <formula1>IF($D11 = "Solid", $C$41:$C$50, IF($D11 = "Liquid", $F$41:$F$50, $I$41:$I$50))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6307,7 +6672,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A12:N20</xm:sqref>
+          <xm:sqref>A12:B20 D12:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{B7FE1704-5B36-4B72-959E-5FFDB77E36BA}">
@@ -6318,7 +6683,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A13:N20</xm:sqref>
+          <xm:sqref>A13:B20 D13:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="8" id="{F763BEC8-2A60-416E-8FF5-218ED81F6E2F}">
@@ -6329,7 +6694,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A14:N20</xm:sqref>
+          <xm:sqref>A14:B20 D14:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{CD6E54D0-86D4-402F-9455-43FE6B6EEE6B}">
@@ -6340,7 +6705,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A15:N20</xm:sqref>
+          <xm:sqref>A15:B20 D15:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="6" id="{685905CA-7FB5-48AF-9084-7E67849A660A}">
@@ -6351,7 +6716,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A16:N20</xm:sqref>
+          <xm:sqref>A16:B20 D16:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="5" id="{82FCB063-5A79-454C-B9F1-3C4A825DD218}">
@@ -6362,7 +6727,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A17:N20</xm:sqref>
+          <xm:sqref>A17:B20 D17:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="4" id="{D446DCEC-CE76-4845-B504-46415EC6D2E9}">
@@ -6373,7 +6738,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A18:N20</xm:sqref>
+          <xm:sqref>A18:B20 D18:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{4354CF35-CD25-434D-AE38-11C3CC645D19}">
@@ -6384,7 +6749,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A19:N20</xm:sqref>
+          <xm:sqref>A19:B20 D19:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="2" id="{69848604-329B-4919-AC1A-B2AE58F4283E}">
@@ -6395,7 +6760,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A20:N20</xm:sqref>
+          <xm:sqref>A20:B20 D20:N20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6406,16 +6771,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C523EF66-94E0-40B7-ABA4-DDB7F41E44FC}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:H31"/>
+  <dimension ref="A2:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="4" width="37.21875" customWidth="1"/>
     <col min="7" max="7" width="37.21875" customWidth="1"/>
     <col min="8" max="8" width="73.6640625" customWidth="1"/>
@@ -6423,222 +6788,228 @@
   <sheetData>
     <row r="2" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="59"/>
+        <v>135</v>
+      </c>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="A3" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="35" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" s="35" customFormat="1" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
+        <v>55</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="H7" s="32" t="s">
         <v>52</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
+        <v>134</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
@@ -6646,16 +7017,16 @@
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
@@ -6663,16 +7034,16 @@
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
@@ -6680,16 +7051,16 @@
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
@@ -6697,63 +7068,99 @@
     </row>
     <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="18"/>
+        <v>168</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+    <row r="20" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" s="16"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="F21" s="16"/>
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>198</v>
+      </c>
       <c r="D23" s="18"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
@@ -6813,14 +7220,768 @@
       <c r="G29" s="20"/>
       <c r="H29" s="21"/>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+    </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
       <c r="G31" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H31" s="22" t="str" cm="1">
-        <f t="array" ref="H31">_xlfn.CONCAT(_xlfn.XLOOKUP(_xlfn.XLOOKUP(TRUE, LogTable[Who?*] &lt;&gt; "", LogTable[Who?*], "¯\_(ツ)_/¯", 0, -1), AuthorTable[Abbr.], AuthorTable[Name], "¯\_(ツ)_/¯", 0, 2), ", ", _xlfn.XLOOKUP(TRUE, LogTable[Date and Time] &lt;&gt; "", LogTable[Date and Time], "¯\_(ツ)_/¯", 0, -1))</f>
-        <v>¯\_(ツ)_/¯, 16/01/2025, 16:18 UTC+7</v>
-      </c>
+        <f t="array" ref="H31">_xlfn.CONCAT(_xlfn.XLOOKUP(_xlfn.XLOOKUP(TRUE, LogTable[Who?*] &lt;&gt; "", LogTable[Who?*], "¯\_(ツ)_/¯", 0, -1), AuthorTable[Abbr.], AuthorTable[Name], "¯\_(ツ)_/¯", 0, 1), ", ", _xlfn.XLOOKUP(TRUE, LogTable[Date and Time] &lt;&gt; "", LogTable[Date and Time], "¯\_(ツ)_/¯", 0, -1))</f>
+        <v>Muhammad Naufal Afif, S.T., 21/08/2025, 21:42 UTC+7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="16"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="16"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="16"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="18"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="18"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="16"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="16"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="16"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="16"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="16"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="18"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="16"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="18"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="16"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="18"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="16"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="18"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="18"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="16"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="18"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="16"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="16"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="16"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="18"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="18"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="18"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="18"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="18"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="16"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="18"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="18"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="16"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="18"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="16"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="18"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="16"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="18"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="16"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="18"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="16"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="18"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="16"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="18"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="16"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="18"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="16"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="18"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="16"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="18"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="16"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="18"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="16"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="18"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="16"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="18"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="16"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="18"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="16"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="18"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="16"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="18"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="16"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="18"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="16"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="18"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="16"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="18"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="16"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="18"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="16"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="18"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="16"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="18"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="16"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="18"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="16"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="18"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="16"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="18"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="16"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="18"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="16"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="18"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="16"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="18"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="16"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="18"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="16"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="18"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="16"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="18"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="16"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="18"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="16"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="18"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="16"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="18"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="16"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="18"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="16"/>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="18"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="16"/>
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="18"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="16"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="18"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="16"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="18"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="16"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="18"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="16"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="18"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="16"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="18"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="16"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="18"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="16"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="18"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="16"/>
+      <c r="B118" s="17"/>
+      <c r="C118" s="17"/>
+      <c r="D118" s="18"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="16"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="18"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="16"/>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="18"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="16"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="18"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="16"/>
+      <c r="B122" s="17"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="18"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="16"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="18"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="16"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="17"/>
+      <c r="D124" s="18"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="16"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="17"/>
+      <c r="D125" s="18"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="16"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="18"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="16"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="18"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="16"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="18"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="16"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="18"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="16"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="18"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="16"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="18"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="16"/>
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="18"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="16"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="18"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="16"/>
+      <c r="B134" s="17"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="18"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="16"/>
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="18"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="16"/>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="18"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="16"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="18"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="16"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="18"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="16"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="18"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="16"/>
+      <c r="B140" s="17"/>
+      <c r="C140" s="17"/>
+      <c r="D140" s="18"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="16"/>
+      <c r="B141" s="17"/>
+      <c r="C141" s="17"/>
+      <c r="D141" s="18"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="16"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="18"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="16"/>
+      <c r="B143" s="17"/>
+      <c r="C143" s="17"/>
+      <c r="D143" s="18"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="16"/>
+      <c r="B144" s="17"/>
+      <c r="C144" s="17"/>
+      <c r="D144" s="18"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="16"/>
+      <c r="B145" s="17"/>
+      <c r="C145" s="17"/>
+      <c r="D145" s="18"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="16"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="18"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="16"/>
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="18"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="16"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="18"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="16"/>
+      <c r="B149" s="17"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="18"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="16"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="18"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="16"/>
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="18"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="16"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="18"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="16"/>
+      <c r="B153" s="17"/>
+      <c r="C153" s="17"/>
+      <c r="D153" s="18"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="16"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="18"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="19"/>
+      <c r="B155" s="20"/>
+      <c r="C155" s="20"/>
+      <c r="D155" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6830,7 +7991,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B29" xr:uid="{7B16103C-6670-42BF-A0DD-7E002CEAB315}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B155" xr:uid="{7B16103C-6670-42BF-A0DD-7E002CEAB315}">
       <formula1>$F$8:$F$29</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>